<commit_message>
perform all LSTM loops and save results
</commit_message>
<xml_diff>
--- a/Assignment 1/LSTM_all_patient_MSEs.xlsx
+++ b/Assignment 1/LSTM_all_patient_MSEs.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69A9740-DD58-437E-819D-D7D2190EB053}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5EF99A-6EB1-4C5D-9D23-A7FE760A9526}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,12 +20,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>stdev</t>
+  </si>
+  <si>
+    <t>CI upper</t>
+  </si>
+  <si>
+    <t>CI lower</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -38,6 +51,14 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,11 +81,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,53 +367,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G4" sqref="G4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0.35950820184885901</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.39544845544847002</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7.5447744366455599E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.59123293802715904</v>
       </c>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.325175892117822</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f>AVERAGE(A1:A27)</f>
+        <v>0.5467001805215147</v>
+      </c>
+      <c r="H5">
+        <f>_xlfn.STDEV.S(A1:A27)</f>
+        <v>0.68889377374396632</v>
+      </c>
+      <c r="I5">
+        <f>$G5 - 2.06*$H5/SQRT(27)</f>
+        <v>0.2735901832644746</v>
+      </c>
+      <c r="J5">
+        <f>$G5 + 2.06*$H5/SQRT(27)</f>
+        <v>0.8198101777785548</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.7110042227159901</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.18735258833593901</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.72751243860433801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.28283518845778499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3.3822950722096401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.56398442220277401</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.110159468313867</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.61004259178938103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.14534333980623601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.63658992736929698</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.152449183550213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.41304446381451798</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.85719014380963199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.120306094137949</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.433660943214076</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.40124965339173202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7.9846545256123905E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.23990679240969201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.102820949700708</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.18565300633019199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.23352373582073199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1.4373208710313199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>